<commit_message>
Add SQL script to fill missing job role values in job_skills table using various methods
</commit_message>
<xml_diff>
--- a/Add_Missing_Values/Problem_Statement.xlsx
+++ b/Add_Missing_Values/Problem_Statement.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thoufiq/THOUFIQ/techTFQ/YouTube/VIDEOS/30 SQL Interview Queries/Video_Q8/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\30DaySQLQueryChallenge - techTFQ\Add_Missing_Values\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{308F00D5-3A79-9342-8F52-DA430DA6D23E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EE980A8-15E7-4139-8C66-A83054750705}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" xr2:uid="{91F0287D-CF68-DD42-BBA9-9FC9563DDF37}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{91F0287D-CF68-DD42-BBA9-9FC9563DDF37}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -90,29 +88,6 @@
   </si>
   <si>
     <t>OUTPUT</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="14"/>
-        <color theme="0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Video #8 </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>- Add the missing values</t>
-    </r>
   </si>
   <si>
     <t>JOB_ROLE</t>
@@ -140,6 +115,29 @@
 In the given input table, there are rows with missing JOB_ROLE values. Write a query to fill in those blank fields with appropriate values.
 Assume row_id is always in sequence and job_role field is populated only for the first skill.
 Provide two different solutions to the problem.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="14"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"># </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>- Add the missing values</t>
     </r>
   </si>
 </sst>
@@ -881,26 +879,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08CDABD5-A95F-A24F-AC54-2A6DF12D3B81}">
   <dimension ref="B1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="2" max="2" width="10.83203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15.83203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17.83203125" style="1" customWidth="1"/>
-    <col min="5" max="6" width="10.83203125" style="1"/>
-    <col min="7" max="7" width="10.83203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="15.83203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="17.83203125" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="10.796875" style="1"/>
+    <col min="2" max="2" width="10.796875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.796875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.796875" style="1" customWidth="1"/>
+    <col min="5" max="6" width="10.796875" style="1"/>
+    <col min="7" max="7" width="10.796875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15.796875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="17.796875" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="10.796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" s="18" customFormat="1" ht="19" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:9" s="18" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="B1" s="21" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C1" s="21"/>
       <c r="D1" s="21"/>
@@ -910,9 +908,9 @@
       <c r="H1" s="21"/>
       <c r="I1" s="21"/>
     </row>
-    <row r="2" spans="2:9" s="19" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:9" s="19" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C2" s="20"/>
       <c r="D2" s="20"/>
@@ -922,7 +920,7 @@
       <c r="H2" s="20"/>
       <c r="I2" s="20"/>
     </row>
-    <row r="3" spans="2:9" s="19" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:9" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B3" s="20"/>
       <c r="C3" s="20"/>
       <c r="D3" s="20"/>
@@ -932,7 +930,7 @@
       <c r="H3" s="20"/>
       <c r="I3" s="20"/>
     </row>
-    <row r="4" spans="2:9" s="19" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:9" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B4" s="20"/>
       <c r="C4" s="20"/>
       <c r="D4" s="20"/>
@@ -942,7 +940,7 @@
       <c r="H4" s="20"/>
       <c r="I4" s="20"/>
     </row>
-    <row r="5" spans="2:9" s="19" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:9" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B5" s="20"/>
       <c r="C5" s="20"/>
       <c r="D5" s="20"/>
@@ -952,7 +950,7 @@
       <c r="H5" s="20"/>
       <c r="I5" s="20"/>
     </row>
-    <row r="6" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
@@ -962,7 +960,7 @@
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
     </row>
-    <row r="7" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="22" t="s">
         <v>16</v>
       </c>
@@ -974,12 +972,12 @@
       <c r="H7" s="26"/>
       <c r="I7" s="27"/>
     </row>
-    <row r="8" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="15" t="s">
         <v>14</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D8" s="17" t="s">
         <v>15</v>
@@ -988,13 +986,13 @@
         <v>14</v>
       </c>
       <c r="H8" s="13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I8" s="14" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B9" s="9">
         <v>1</v>
       </c>
@@ -1014,7 +1012,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B10" s="4">
         <v>2</v>
       </c>
@@ -1032,7 +1030,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B11" s="4">
         <v>3</v>
       </c>
@@ -1050,7 +1048,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B12" s="4">
         <v>4</v>
       </c>
@@ -1068,7 +1066,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B13" s="4">
         <v>5</v>
       </c>
@@ -1086,7 +1084,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B14" s="4">
         <v>6</v>
       </c>
@@ -1106,7 +1104,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B15" s="4">
         <v>7</v>
       </c>
@@ -1124,7 +1122,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B16" s="4">
         <v>8</v>
       </c>
@@ -1142,7 +1140,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B17" s="4">
         <v>9</v>
       </c>
@@ -1162,7 +1160,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B18" s="4">
         <v>10</v>
       </c>
@@ -1180,7 +1178,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B19" s="4">
         <v>11</v>
       </c>
@@ -1198,7 +1196,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B20" s="6">
         <v>12</v>
       </c>
@@ -1224,5 +1222,6 @@
     <mergeCell ref="G7:I7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>